<commit_message>
added COT data from Zhu paper
</commit_message>
<xml_diff>
--- a/UUVPerformance.xlsx
+++ b/UUVPerformance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Propeller" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="114">
   <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
@@ -310,6 +310,24 @@
     <t xml:space="preserve">https://doi.org/10.1109/IROS.2014.6942574</t>
   </si>
   <si>
+    <t xml:space="preserve">NTNU Mamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCSD DEA leptocephali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christianson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of California, San Diego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1126/scirobotics.aat1893</t>
+  </si>
+  <si>
     <t xml:space="preserve">UV Robotic Mantaray</t>
   </si>
   <si>
@@ -323,6 +341,15 @@
   </si>
   <si>
     <t xml:space="preserve">http://brcl.me.uh.edu/Paper/JSMN11.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UV Cownose Ray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.researchgate.net/publication/266891803_Bio-Inspired_Robotic_Cownose_Ray_Propelled_by_Electroactive_Polymer_Pectoral_Fin</t>
   </si>
   <si>
     <t xml:space="preserve">Madeline</t>
@@ -540,7 +567,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -571,10 +598,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -617,19 +640,12 @@
     <cellStyle name="Text 13" xfId="29"/>
     <cellStyle name="Warning 14" xfId="30"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <fgColor rgb="FFFCFCFC"/>
+          <bgColor rgb="FF1B1E20"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1130,7 +1146,7 @@
         <f aca="false">(I4*D4)/0.000001</f>
         <v>1203242.04744049</v>
       </c>
-      <c r="O4" s="8" t="n">
+      <c r="O4" s="1" t="n">
         <v>1508028.96725441</v>
       </c>
       <c r="P4" s="1" t="n">
@@ -1232,14 +1248,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V11" activeCellId="0" sqref="V11"/>
+      <selection pane="bottomRight" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1272,98 +1288,98 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="74" style="1" width="8.62"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2078,7 +2094,150 @@
         <v>94</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <f aca="false">Q11/L11</f>
+        <v>64.8145833333333</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <f aca="false">O11/9.81</f>
+        <v>6.6069911654774</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>933.33</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <f aca="false">Q11*I11</f>
+        <v>1493.328</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>2.093</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <f aca="false">N11*I11/0.000001</f>
+        <v>120000</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <f aca="false">(4*PI()*S11*T11*I11^2)/0.000001</f>
+        <v>8416452.3826732</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>0.0251</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>0.0019</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>0.0019</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <f aca="false">Q12/L12</f>
+        <v>418.326693227092</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <f aca="false">O12/9.81</f>
+        <v>42.6428841210083</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <f aca="false">Q12*I12</f>
+        <v>2.31</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <f aca="false">N12*I12/0.000001</f>
+        <v>418</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <f aca="false">(4*PI()*S12*T12*I12^2)/0.000001</f>
+        <v>10035.5035726272</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AE12" r:id="rId1" display="https://doi.org/10.1126/scirobotics.aat1893"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2087,7 +2246,7 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2097,203 +2256,282 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="24.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="16.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="29.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="11" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="11" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="14" style="11" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="11" width="23.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="11" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="12" width="21.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="11" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="12" width="13.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="11" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="27" style="11" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="24.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="16.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="29.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="10" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="10" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="10" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="14" style="10" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="10" width="23.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="10" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="11" width="21.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="10" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="11" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="10" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="27" style="10" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="71" style="1" width="8.62"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AB1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AC1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AD1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="11" t="n">
+      <c r="D2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="10" t="n">
         <f aca="false">F2</f>
         <v>2</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="10" t="n">
         <v>0.11</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="10" t="n">
         <v>0.21</v>
       </c>
-      <c r="J2" s="11" t="n">
+      <c r="J2" s="10" t="n">
         <v>0.025</v>
       </c>
-      <c r="K2" s="11" t="n">
+      <c r="K2" s="10" t="n">
         <v>0.055</v>
       </c>
-      <c r="L2" s="11" t="n">
+      <c r="L2" s="10" t="n">
         <v>0.0074</v>
       </c>
-      <c r="M2" s="11" t="n">
+      <c r="M2" s="10" t="n">
         <v>0.00737</v>
       </c>
-      <c r="N2" s="11" t="n">
+      <c r="N2" s="10" t="n">
         <f aca="false">P2/K2</f>
         <v>6167.45454545455</v>
       </c>
-      <c r="O2" s="11" t="n">
+      <c r="O2" s="10" t="n">
         <f aca="false">N2/9.81</f>
         <v>628.690575479566</v>
       </c>
-      <c r="P2" s="11" t="n">
+      <c r="P2" s="10" t="n">
         <v>339.21</v>
       </c>
-      <c r="Q2" s="11" t="n">
+      <c r="Q2" s="10" t="n">
         <f aca="false">P2*H2</f>
         <v>37.3131</v>
       </c>
-      <c r="R2" s="11" t="n">
+      <c r="R2" s="10" t="n">
         <v>0.167</v>
       </c>
-      <c r="S2" s="11" t="n">
+      <c r="S2" s="10" t="n">
         <v>0.20238</v>
       </c>
-      <c r="T2" s="11" t="n">
+      <c r="T2" s="10" t="n">
         <f aca="false">(H2*M2)/0.000001</f>
         <v>810.7</v>
       </c>
-      <c r="U2" s="11" t="n">
+      <c r="U2" s="10" t="n">
         <f aca="false">(4*PI()*R2*S2*H2^2)/0.000001</f>
         <v>5139.00803902615</v>
       </c>
-      <c r="Z2" s="13"/>
-      <c r="AD2" s="11" t="s">
-        <v>99</v>
+      <c r="Z2" s="12"/>
+      <c r="AD2" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <f aca="false">F3</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I3" s="10" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J3" s="10" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K3" s="10" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <f aca="false">L3</f>
+        <v>0.07</v>
+      </c>
+      <c r="N3" s="10" t="n">
+        <f aca="false">P3/K3</f>
+        <v>2352.94117647059</v>
+      </c>
+      <c r="O3" s="10" t="n">
+        <f aca="false">N3/9.81</f>
+        <v>239.851292198837</v>
+      </c>
+      <c r="P3" s="10" t="n">
+        <v>280</v>
+      </c>
+      <c r="Q3" s="10" t="n">
+        <f aca="false">P3*H3</f>
+        <v>58.8</v>
+      </c>
+      <c r="R3" s="10" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="S3" s="10" t="n">
+        <v>0.010332</v>
+      </c>
+      <c r="T3" s="10" t="n">
+        <f aca="false">(H3*M3)/0.000001</f>
+        <v>14700</v>
+      </c>
+      <c r="U3" s="10" t="n">
+        <f aca="false">(4*PI()*R3*S3*H3^2)/0.000001</f>
+        <v>898.943721260302</v>
+      </c>
+      <c r="Z3" s="12"/>
+      <c r="AB3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2317,239 +2555,239 @@
   </sheetPr>
   <dimension ref="A1:BQ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="16.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="29.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="11" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="11" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="14" style="11" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="11" width="23.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="11" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="12" width="13.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="11" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="12" width="13.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="13" width="45.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="27" style="11" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="13" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="16.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="29.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="10" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="10" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="10" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="14" style="10" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="10" width="23.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="10" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="11" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="10" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="11" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="12" width="45.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="27" style="10" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="12" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AB1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AC1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AD1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="13"/>
-      <c r="BO1" s="13"/>
-      <c r="BP1" s="13"/>
-      <c r="BQ1" s="13"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12"/>
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="A2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="11" t="n">
+      <c r="F2" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="10" t="n">
         <f aca="false">F2</f>
         <v>4</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="10" t="n">
         <v>0.78</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="10" t="n">
         <v>0.44</v>
       </c>
-      <c r="J2" s="11" t="n">
+      <c r="J2" s="10" t="n">
         <v>0.13</v>
       </c>
-      <c r="K2" s="11" t="n">
+      <c r="K2" s="10" t="n">
         <v>24.4</v>
       </c>
-      <c r="L2" s="11" t="n">
+      <c r="L2" s="10" t="n">
         <v>0.77</v>
       </c>
-      <c r="M2" s="11" t="n">
+      <c r="M2" s="10" t="n">
         <v>0.77</v>
       </c>
-      <c r="N2" s="11" t="n">
+      <c r="N2" s="10" t="n">
         <f aca="false">P2/K2</f>
         <v>3.4335</v>
       </c>
-      <c r="O2" s="11" t="n">
+      <c r="O2" s="10" t="n">
         <f aca="false">N2/9.81</f>
         <v>0.35</v>
       </c>
-      <c r="P2" s="11" t="n">
+      <c r="P2" s="10" t="n">
         <v>83.7774</v>
       </c>
-      <c r="Q2" s="11" t="n">
+      <c r="Q2" s="10" t="n">
         <f aca="false">P2*H2</f>
         <v>65.346372</v>
       </c>
-      <c r="R2" s="11" t="n">
+      <c r="R2" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="S2" s="11" t="n">
+      <c r="S2" s="10" t="n">
         <v>0.0288</v>
       </c>
-      <c r="T2" s="11" t="n">
+      <c r="T2" s="10" t="n">
         <f aca="false">(M2*H2)/0.000001</f>
         <v>600600</v>
       </c>
-      <c r="U2" s="11" t="n">
+      <c r="U2" s="10" t="n">
         <f aca="false">(4*PI()*R2*S2*H2^2)/0.000001</f>
         <v>1321121.64357091</v>
       </c>
-      <c r="AD2" s="13" t="s">
-        <v>104</v>
+      <c r="AD2" s="12" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>